<commit_message>
Bug fixes to the marmot function, namely rendering to HTML.
</commit_message>
<xml_diff>
--- a/MARMOT_Metadata.xlsx
+++ b/MARMOT_Metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterleary/Desktop/IMCR/MARMOT/For_Submission/MARMOT_Paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterleary/Desktop/FGCZ/MARMOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A8B14-68E8-B94E-8BA6-7D7C8BC4AAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880E65D8-CE34-A649-92FA-7093F2C969C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3460" yWindow="2760" windowWidth="39400" windowHeight="21660" xr2:uid="{9C611E3C-4644-F449-9441-E60F328909FC}"/>
   </bookViews>
@@ -420,9 +420,6 @@
     <t xml:space="preserve">Enter the number of processor cores the pipeline can use. Don’t use all! </t>
   </si>
   <si>
-    <t xml:space="preserve">Enter an amount of RAM per processor core. Marmot likes at least 6. </t>
-  </si>
-  <si>
     <t>prism</t>
   </si>
   <si>
@@ -438,12 +435,6 @@
     <t>void</t>
   </si>
   <si>
-    <t>Select a ggplot theme to use. We suggest prism.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select a viridis theme to use. We suggest mako. </t>
-  </si>
-  <si>
     <t>viridis</t>
   </si>
   <si>
@@ -496,6 +487,15 @@
   </si>
   <si>
     <t xml:space="preserve">Enter a number to downsample to when calculating DR plots. Leave blank to include all cells. </t>
+  </si>
+  <si>
+    <t>Enter an amount of RAM per processor core. Marmot likes at least 6. Make sure nCores*ramPerCore is less than your total amount of RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a viridis theme to use. Marmots like mako. </t>
+  </si>
+  <si>
+    <t>Select a ggplot theme to use. Marmots like prism.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,6 +583,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -731,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,67 +748,126 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -820,6 +885,18 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -829,6 +906,36 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -868,56 +975,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -932,12 +989,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:C22" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1243,21 +1300,21 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="128.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1265,24 +1322,24 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="12">
         <v>1000</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>148</v>
+      <c r="C2" s="13" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="16" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1290,10 +1347,10 @@
       <c r="A4" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="16" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1301,10 +1358,10 @@
       <c r="A5" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1312,189 +1369,189 @@
       <c r="A6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="15">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="16" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="19" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="19" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="24">
+        <v>4</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="24">
+        <v>6</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="10" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="27">
-        <v>4</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="27">
-        <v>6</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1574,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14367E5-7343-7A4C-8EFF-60584647CF54}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1946,7 +2003,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2154,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2174,10 +2231,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2191,10 +2248,10 @@
         <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2202,33 +2259,33 @@
         <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed a variable name because it was confusing apparently -.-
</commit_message>
<xml_diff>
--- a/MARMOT_Metadata.xlsx
+++ b/MARMOT_Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterleary/Desktop/FGCZ/MARMOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880E65D8-CE34-A649-92FA-7093F2C969C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C9C21E-A2CB-6046-B898-14DAA7ECE097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3460" yWindow="2760" windowWidth="39400" windowHeight="21660" xr2:uid="{9C611E3C-4644-F449-9441-E60F328909FC}"/>
   </bookViews>
@@ -324,9 +324,6 @@
     <t>runQC</t>
   </si>
   <si>
-    <t>removeFromQC</t>
-  </si>
-  <si>
     <t>useQC</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>~/Desktop/MARMOT/</t>
   </si>
   <si>
-    <t>Enter one or more of FR (flow rate), FS (signal acquisition), and FM (dynamic range), space separated.</t>
-  </si>
-  <si>
     <t>FR FS</t>
   </si>
   <si>
@@ -496,6 +490,12 @@
   </si>
   <si>
     <t>Select a ggplot theme to use. Marmots like prism.</t>
+  </si>
+  <si>
+    <t>Enter one or more of FR (flow rate), FS (signal acquisition), and FM (dynamic range) to QC with flowAI, space separated.</t>
+  </si>
+  <si>
+    <t>metricsQC</t>
   </si>
 </sst>
 </file>
@@ -761,74 +761,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -935,6 +921,20 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -989,12 +989,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C22" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,13 +1312,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1329,7 +1329,7 @@
         <v>1000</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1337,10 +1337,10 @@
         <v>84</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1348,10 +1348,10 @@
         <v>85</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1359,10 +1359,10 @@
         <v>86</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1373,7 +1373,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1381,10 +1381,10 @@
         <v>88</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1395,7 +1395,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1415,115 +1415,115 @@
         <v>1</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="21" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="24">
         <v>4</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="24">
         <v>6</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1531,10 +1531,10 @@
         <v>81</v>
       </c>
       <c r="B21" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>139</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1542,10 +1542,10 @@
         <v>82</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2199,93 +2199,93 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D1" t="b">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fix to marmot function to properly source the rmd
</commit_message>
<xml_diff>
--- a/MARMOT_Metadata.xlsx
+++ b/MARMOT_Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterleary/Desktop/FGCZ/MARMOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C9C21E-A2CB-6046-B898-14DAA7ECE097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AF043D-402B-2248-96BB-4D0A8FAE27FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3460" yWindow="2760" windowWidth="39400" windowHeight="21660" xr2:uid="{9C611E3C-4644-F449-9441-E60F328909FC}"/>
   </bookViews>
@@ -324,6 +324,9 @@
     <t>runQC</t>
   </si>
   <si>
+    <t>removeFromQC</t>
+  </si>
+  <si>
     <t>useQC</t>
   </si>
   <si>
@@ -474,6 +477,9 @@
     <t>~/Desktop/MARMOT/</t>
   </si>
   <si>
+    <t>Enter one or more of FR (flow rate), FS (signal acquisition), and FM (dynamic range), space separated.</t>
+  </si>
+  <si>
     <t>FR FS</t>
   </si>
   <si>
@@ -490,12 +496,6 @@
   </si>
   <si>
     <t>Select a ggplot theme to use. Marmots like prism.</t>
-  </si>
-  <si>
-    <t>Enter one or more of FR (flow rate), FS (signal acquisition), and FM (dynamic range) to QC with flowAI, space separated.</t>
-  </si>
-  <si>
-    <t>metricsQC</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -989,12 +999,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:C22" xr:uid="{3586C4B2-ADB2-8944-8759-A59E39853E12}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6E5D9E7E-2965-C342-935C-46AFF40862A4}" name="Variable" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3651CB78-AF61-9F48-9271-E82C28D1865F}" name="Setting" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9A550912-B61D-BA41-87DB-136B1A08B9E2}" name="Info" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1300,7 +1310,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,13 +1322,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1329,7 +1339,7 @@
         <v>1000</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1337,10 +1347,10 @@
         <v>84</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1348,10 +1358,10 @@
         <v>85</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1359,10 +1369,10 @@
         <v>86</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1373,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1381,10 +1391,10 @@
         <v>88</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1395,7 +1405,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1404,7 +1414,7 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1415,115 +1425,115 @@
         <v>1</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B12" s="21" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B15" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B16" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17" s="24">
         <v>4</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B18" s="24">
         <v>6</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1531,10 +1541,10 @@
         <v>81</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1542,10 +1552,10 @@
         <v>82</v>
       </c>
       <c r="B22" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="31" t="s">
         <v>141</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1554,6 +1564,11 @@
       <c r="C23" s="9"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK(A3)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2199,93 +2214,93 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" t="b">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>